<commit_message>
Pics of diagramms updated
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Documents\ITTimeRecording\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="580" windowWidth="23260" windowHeight="11950"/>
+    <workbookView xWindow="240" yWindow="585" windowWidth="23265" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>№</t>
   </si>
@@ -78,15 +73,6 @@
     <t>Активность текущего рабочего дня изменяется на выбранную</t>
   </si>
   <si>
-    <t>Перенос рабочего дня разработчиком</t>
-  </si>
-  <si>
-    <t>Пользователь авторизован как разработчик и хочет перенести рабочий день</t>
-  </si>
-  <si>
-    <t>Перенесенный рабочий день для данного сотрудника становится выходным, а день, на который произошел перенос - рабочим</t>
-  </si>
-  <si>
     <t>Заказ переработки разрабочиком</t>
   </si>
   <si>
@@ -96,33 +82,12 @@
     <t>День, приходящийся на дату переработки становится рабочим</t>
   </si>
   <si>
-    <t>Регистрация сотрудника HR'ом</t>
-  </si>
-  <si>
     <t>Пользователь авторизован как HR и хочет зарегистрировать сотрудника</t>
   </si>
   <si>
     <t>Новый пользователь появляется в системе</t>
   </si>
   <si>
-    <t>Просмотр информации о сотруднике HR'ом</t>
-  </si>
-  <si>
-    <t>Пользователь авторизован как HR и хочет просмотреть информацию о сотруднике</t>
-  </si>
-  <si>
-    <t>Показывается информация о пользователе</t>
-  </si>
-  <si>
-    <t>Просмотр резюме HR'ом</t>
-  </si>
-  <si>
-    <t>Пользователь авторизован как HR и хочет просмотреть резюме</t>
-  </si>
-  <si>
-    <t>Показывается резюме (ссылка на pdf файл) и кнопка Далее</t>
-  </si>
-  <si>
     <t>Смена активности сотрудника менеджером</t>
   </si>
   <si>
@@ -136,33 +101,6 @@
   </si>
   <si>
     <t>Пользователь авторизован как менеджер и хочет проконтролировать рабочий день сотрудника</t>
-  </si>
-  <si>
-    <t>Смена активности сотрудника топ-менеджером</t>
-  </si>
-  <si>
-    <t>Пользователь авторизован как топ-менеджер и хочет поменять активность для сотрудника</t>
-  </si>
-  <si>
-    <t>Контроль рабочего дня сотрудника топ-менеджером</t>
-  </si>
-  <si>
-    <t>Пользователь авторизован как топ-менеджер и хочет проконтролировать рабочий день сотрудника</t>
-  </si>
-  <si>
-    <t>Смена коэффициентов активности топ-менеджером</t>
-  </si>
-  <si>
-    <t>Пользователь авторизован как топ-менеджер и хочет поменять коэффициенты активности для сотрудника</t>
-  </si>
-  <si>
-    <t>Коэффициент активности сотрудника изменяется на выбранный</t>
-  </si>
-  <si>
-    <t>Пользователь авторизован как топ-менеджер и хочет поменять коэффициенты проекта для сотрудника</t>
-  </si>
-  <si>
-    <t>Коэффициент проекта сотрудника изменяется на выбранный</t>
   </si>
   <si>
     <t>1. Выполнение сценария 1.1 
@@ -176,21 +114,6 @@
 4. Пользователь нажимает на кнопку подтверждения</t>
   </si>
   <si>
-    <t>1. Выполнение сценария 1.1 HR'ом
-2. Пользователь выбирает соответствующий пункт на главной странице
-3. Пользователь вводит данные о регистрируемом сотруднике в форму
-4. Пользователь нажимает кнопку подтверждения</t>
-  </si>
-  <si>
-    <t>1. Выполнение сценария 1.1 HR'ом
-2. Пользователь выбирает соответствующий пункт на главной странице 
-3. Пользователь вводит данные о пользователе в поле поиска</t>
-  </si>
-  <si>
-    <t>1. Выполнение сценария 1.1 HR'ом
-2. Пользователь выбирает соответствующий пункт на главной странице</t>
-  </si>
-  <si>
     <t>1. Выполнение сценария 1.1 менеджером
 2. Пользователь выбирает соответствующий пункт на главной странице
 3. Пользователь выбирает активность для сотрудника 
@@ -203,39 +126,19 @@
 4. Пользователь начинает или заканчивает рабочий день сотрудника, нажимая соответствующие кнопки</t>
   </si>
   <si>
-    <t>1. Выполнение сценария 1.1 топ-менеджером
+    <t>Регистрация сотрудника менеджером</t>
+  </si>
+  <si>
+    <t>1. Выполнение сценария 1.1 менеджером
 2. Пользователь выбирает соответствующий пункт на главной странице
-3. Пользователь выбирает активность 
-4. Пользователь изменяет значение коэффициента
-5. Пользователь после чего нажимает кнопку подтверждения</t>
-  </si>
-  <si>
-    <t>1. Выполнение сценария 1.1 топ-менеджером
-2. Пользователь выбирает соответствующий пункт на главной странице
-3. Пользователь выбирает проект 
-4. Пользователь изменяет значение коэффициента
-5. Пользователь после чего нажимает кнопку подтверждения</t>
-  </si>
-  <si>
-    <t>1. Выполнение сценария 1.1 топ-менеджером
-2. Пользователь выбирает соответствующий пункт на главной странице 
-3. Пользователь выбирает сотрудника 
-4. Пользователь начинает или заканчивает рабочий день сотрудника, нажимая соответствующие кнопки</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Выполнение сценария 1.1 разработчиком
-2. Пользователь выбирает пункт меню соответствующий переносу рабочего дня на главной странице
-3. Пользователь выбирает даты (откуда переносит и куда) с помощью формы
-4. Пользователь нажимает на кнопку подтверждения. </t>
-  </si>
-  <si>
-    <t>Смена коэффициентов проекта топ-менеджером</t>
+3. Пользователь вводит данные о регистрируемом сотруднике в форму
+4. Пользователь нажимает кнопку подтверждения</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
@@ -279,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -315,11 +218,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -340,6 +271,42 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -402,7 +369,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -434,10 +401,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -469,7 +435,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -645,26 +610,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.90625" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
-    <col min="5" max="5" width="30.6328125" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25">
+    <row r="1" spans="1:7" ht="25.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +652,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="37.5">
+    <row r="2" spans="1:7" ht="38.25">
       <c r="A2" s="2">
         <v>43466</v>
       </c>
@@ -706,7 +671,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:7" ht="37.5">
+    <row r="3" spans="1:7" ht="38.25">
       <c r="A3" s="2">
         <v>43497</v>
       </c>
@@ -725,7 +690,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" spans="1:7" ht="37.5">
+    <row r="4" spans="1:7" ht="51">
       <c r="A4" s="2">
         <v>43525</v>
       </c>
@@ -736,7 +701,7 @@
         <v>16</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>47</v>
+        <v>28</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>17</v>
@@ -744,7 +709,7 @@
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
-    <row r="5" spans="1:7" ht="75">
+    <row r="5" spans="1:7" ht="76.5">
       <c r="A5" s="2">
         <v>43467</v>
       </c>
@@ -755,7 +720,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>20</v>
@@ -763,195 +728,98 @@
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
-    <row r="6" spans="1:7" ht="75">
+    <row r="6" spans="1:7" ht="76.5">
       <c r="A6" s="2">
-        <v>43498</v>
-      </c>
-      <c r="B6" s="3" t="s">
+        <v>43468</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
-    <row r="7" spans="1:7" ht="75">
-      <c r="A7" s="2">
-        <v>43468</v>
-      </c>
-      <c r="B7" s="6" t="s">
+    <row r="7" spans="1:7" ht="63.75">
+      <c r="A7" s="8">
+        <v>43499</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="76.5">
+      <c r="A8" s="16">
+        <v>43527</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:7" ht="50">
-      <c r="A8" s="2">
-        <v>43499</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:7" ht="37.5">
-      <c r="A9" s="2">
-        <v>43527</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="D8" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:7" ht="62.5">
-      <c r="A10" s="2">
-        <v>43469</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="75">
-      <c r="A11" s="2">
-        <v>43500</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="E8" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:7" ht="75">
-      <c r="A12" s="2">
-        <v>43470</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:7" ht="75">
-      <c r="A13" s="2">
-        <v>43501</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:7" ht="75">
-      <c r="A14" s="2">
-        <v>43529</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:7" ht="75">
-      <c r="A15" s="2">
-        <v>43560</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+    </row>
+    <row r="9" spans="1:7" ht="18">
+      <c r="A9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:7" ht="18">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:7" ht="18">
+      <c r="A11" s="12"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+    </row>
+    <row r="12" spans="1:7" ht="18">
+      <c r="A12" s="12"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Screenshots inserted into course project and new test-cases added
</commit_message>
<xml_diff>
--- a/Testing.xlsx
+++ b/Testing.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Documents\ITTimeRecording\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="590" windowWidth="23270" windowHeight="11960"/>
+    <workbookView xWindow="240" yWindow="585" windowWidth="23265" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>№</t>
   </si>
@@ -176,26 +171,109 @@
     <t>Активность выбранного пользователя успешно изменена</t>
   </si>
   <si>
-    <t>Не пройдено</t>
-  </si>
-  <si>
-    <t>Функционал не доработан</t>
-  </si>
-  <si>
-    <t>Пройдено с недочетами</t>
-  </si>
-  <si>
-    <t>Время сбрасывается при параллельном выполнении сценария для разных пользователей</t>
+    <t>Изменение типа дня осуществелено</t>
+  </si>
+  <si>
+    <t>1.1.1.</t>
+  </si>
+  <si>
+    <t>Негативный сценарий авторизации пользователя</t>
+  </si>
+  <si>
+    <t>Ввод неверных данных при авторизации</t>
+  </si>
+  <si>
+    <t>1. Ввод неверных логина или пароля
+2. Нажатие на кнопку подтверждения</t>
+  </si>
+  <si>
+    <t>Время высчитывается корректно</t>
+  </si>
+  <si>
+    <t>Предупреждение пользователя об ошибке посредством сообщения</t>
+  </si>
+  <si>
+    <t>Сообщение об ошибке высветилось</t>
+  </si>
+  <si>
+    <t>2.1.1.</t>
+  </si>
+  <si>
+    <t>Негативный сценарий заказа переработки разработчиком</t>
+  </si>
+  <si>
+    <t>Заказ переработки на прежде заказанный выходной</t>
+  </si>
+  <si>
+    <t>1. Выполнение сценария 1.1 разработчиком
+2. Пользователь заказывает выходной, нажав на дату календаря
+3. Пользователь заказывает переработку, нажав на дату календаря, задействованную в пункте 2.</t>
+  </si>
+  <si>
+    <t>Активность выбранного рабочего дня становится стандартной вместо переработки</t>
+  </si>
+  <si>
+    <t>Активность выбранного рабочего дня стала стандартной</t>
+  </si>
+  <si>
+    <t>Негативный сценарий регистрации сотрудника менеджером</t>
+  </si>
+  <si>
+    <t>Пользователь авторизован как менеджер и хочет зарегистрировать уже существующего сотрудника</t>
+  </si>
+  <si>
+    <t>1. Выполнение сценария 1.1 менеджером
+2. Пользователь выбирает соответствующий пункт на главной странице
+3. Пользователь вводит данные о существующем сотруднике в форму
+4. Пользователь нажимает кнопку подтверждения</t>
+  </si>
+  <si>
+    <t>3.1.1.</t>
+  </si>
+  <si>
+    <t>0.0.0.</t>
+  </si>
+  <si>
+    <t>Попытка перейти на URL, который не соответствует выбранной роли</t>
+  </si>
+  <si>
+    <t>Пользователь ввел URL, не соответсвующий его роли</t>
+  </si>
+  <si>
+    <t>1. Выполнение сценария 1.1 разработчиком
+2. Ввод URL, соотвествующего шаблону /manager/{action}</t>
+  </si>
+  <si>
+    <t>Пользователь возвращается на свою домашнюю страницу</t>
+  </si>
+  <si>
+    <t>Перенаправления на страницу менеджера не произошло</t>
+  </si>
+  <si>
+    <t>Пользователь ввел URL, не предусмотренный приложением</t>
+  </si>
+  <si>
+    <t>1. Выполнение сценария 1.1 пользователем
+2. Ввод URL , не предусмотренного приложением</t>
+  </si>
+  <si>
+    <t>Пользователь перенаправляется на страницу ошибки 404</t>
+  </si>
+  <si>
+    <t>Высвечивается страница 404</t>
+  </si>
+  <si>
+    <t>Попытка перейти на несуществующий URL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -233,8 +311,15 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -255,18 +340,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="2"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -330,15 +433,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -369,18 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -414,11 +515,44 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -480,7 +614,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -512,10 +646,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -547,7 +680,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Стандартная">
@@ -723,270 +855,350 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.81640625" customWidth="1"/>
-    <col min="2" max="2" width="19.453125" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
     <col min="3" max="3" width="26" customWidth="1"/>
     <col min="4" max="4" width="55" customWidth="1"/>
-    <col min="5" max="5" width="30.54296875" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="25.5">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="34" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="37.5">
-      <c r="A2" s="2">
+    <row r="2" spans="1:7" ht="38.25">
+      <c r="A2" s="1">
         <v>43466</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="37.5">
-      <c r="A3" s="2">
+    <row r="3" spans="1:7" ht="38.25">
+      <c r="A3" s="1">
         <v>43497</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="15" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="50">
-      <c r="A4" s="2">
+    <row r="4" spans="1:7" ht="51">
+      <c r="A4" s="1">
         <v>43525</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="75">
-      <c r="A5" s="2">
+    <row r="5" spans="1:7" ht="76.5">
+      <c r="A5" s="1">
         <v>43467</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="6" t="s">
+    </row>
+    <row r="6" spans="1:7" ht="76.5">
+      <c r="A6" s="1">
+        <v>43468</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="63.75">
+      <c r="A7" s="7">
+        <v>43499</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="63.75">
+      <c r="A8" s="7">
+        <v>43527</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="76.5">
+      <c r="A9" s="11">
+        <v>43558</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="51">
+      <c r="A10" s="22" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="75">
-      <c r="A6" s="2">
-        <v>43468</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F6" s="21" t="s">
+      <c r="B10" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="62.5">
-      <c r="A7" s="8">
-        <v>43499</v>
-      </c>
-      <c r="B7" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="23" t="s">
+      <c r="G10" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="63.75">
+      <c r="A11" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="24" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="62.5">
-      <c r="A8" s="8">
-        <v>43527</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="23" t="s">
+      <c r="G11" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="76.5">
+      <c r="A12" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="G8" s="24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="100">
-      <c r="A9" s="16">
-        <v>43558</v>
-      </c>
-      <c r="B9" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="18">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-    </row>
-    <row r="11" spans="1:7" ht="18">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-    </row>
-    <row r="12" spans="1:7" ht="18">
-      <c r="A12" s="12"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="13" spans="1:7" ht="18">
-      <c r="A13" s="12"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
+      <c r="G12" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="51">
+      <c r="A13" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" customHeight="1">
+      <c r="A14" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" s="33" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="31" t="s">
+        <v>72</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>